<commit_message>
last commit before PUSHING to remote GITHUB
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -468,7 +468,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>117.84</v>
+        <v>119.05</v>
       </c>
       <c r="C2" t="n">
         <v>90.94</v>
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>211.75</v>
+        <v>214.07</v>
       </c>
       <c r="C3" t="n">
         <v>136.53</v>

</xml_diff>